<commit_message>
added test case in each sprint
</commit_message>
<xml_diff>
--- a/document/4.Prpject Plan/Test Case/[URs] Test case_Sprint 4_v1.0 .xlsx
+++ b/document/4.Prpject Plan/Test Case/[URs] Test case_Sprint 4_v1.0 .xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Nam_4\Capstone 1\Source Code\university-reviews-fe\document\4.Prpject Plan\Test Case\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="135" yWindow="510" windowWidth="20730" windowHeight="10530"/>
   </bookViews>
   <sheets>
     <sheet name="Chỉnh sửa thông tin cá nhân" sheetId="8" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Hiện thị đúng thiết kế</t>
   </si>
@@ -64,57 +69,7 @@
     <t>Test case Cập nhật thông tin cá nhân</t>
   </si>
   <si>
-    <t>1. Để trống Tên người dùng
-2. Để trống Giới tính
-3. Để trống Email hoặc Số điện thoại
-4. Để trống Mô tả thông tin
-5. Để trống Mật khẩu
-6. Để trống Nhập lại mật khẩu
-7. Không Upload Ảnh
-8. Click nút Cập nhật</t>
-  </si>
-  <si>
     <t>Hiển thị thông báo nhập những thông tin bắt buộc</t>
-  </si>
-  <si>
-    <t>1. Nhập đúng Tên người dùng
-2. Để trống Giới tính
-3. Để trống Email hoặc Số điện thoại
-4. Để trống Mô tả thông tin
-5. Để trống Mật khẩu
-6. Để trống Nhập lại mật khẩu
-7. Không Upload Ảnh
-8. Click nút Cập nhật</t>
-  </si>
-  <si>
-    <t>1. Nhập đúng Tên người dùng
-2. Chọn Giới tính
-3. Để trống Email hoặc Số điện thoại
-4. Để trống Mô tả thông tin
-5. Để trống Mật khẩu
-6. Để trống Nhập lại mật khẩu
-7. Không Upload Ảnh
-8. Click nút Cập nhật</t>
-  </si>
-  <si>
-    <t>1. Nhập đúng Tên người dùng
-2. Chọn Giới tính
-3. Nhập đúng Email hoặc Số điện thoại
-4. Để trống Mô tả thông tin
-5. Để trống Mật khẩu
-6. Để trống Nhập lại mật khẩu
-7. Không Upload Ảnh
-8. Click nút Cập nhật</t>
-  </si>
-  <si>
-    <t>1. Nhập đúng Tên người dùng
-2. Chọn Giới tính
-3. Nhập đúng Email hoặc Số điện thoại
-4. Nhập đúng Mô tả thông tin
-5. Để trống Mật khẩu
-6. Để trống Nhập lại mật khẩu
-7. Không Upload Ảnh
-8. Click nút Cập nhật</t>
   </si>
   <si>
     <t>1. Nhập đúng Tên người dùng
@@ -130,40 +85,10 @@
     <t>Hiển thị thông báo Nhập lại mật khẩu</t>
   </si>
   <si>
-    <t>1. Nhập đúng Tên người dùng
-2. Chọn Giới tính
-3. Nhập đúng Email hoặc Số điện thoại
-4. Nhập đúng Mô tả thông tin
-5. Nhập đúng Mật khẩu
-6. Nhập đúng Nhập lại mật khẩu
-7. Không Upload Ảnh
-8. Click nút Cập nhật</t>
-  </si>
-  <si>
     <t>Hiển thị thông báo Upload Ảnh</t>
   </si>
   <si>
-    <t>1. Nhập đúng Tên người dùng
-2. Chọn Giới tính
-3. Nhập đúng Email hoặc Số điện thoại
-4. Nhập đúng Mô tả thông tin
-5. Nhập đúng Mật khẩu
-6. Nhập đúng Nhập lại mật khẩu
-7. Upload Ảnh
-8. Click nút Cập nhật</t>
-  </si>
-  <si>
     <t>Hiển thị thông báo Cập nhật thành công</t>
-  </si>
-  <si>
-    <t>1. Nhập đúng Tên người dùng
-2. Chọn Giới tính
-3. Nhập sai Email hoặc Số điện thoại
-4. Nhập đúng Mô tả thông tin
-5. Nhập đúng Mật khẩu
-6. Nhập đúng Nhập lại mật khẩu
-7. Upload Ảnh
-8. Click nút Cập nhật</t>
   </si>
   <si>
     <t>Hiển thị thông báo Email hoặc Số điện thoại sai định dạng</t>
@@ -171,11 +96,65 @@
   <si>
     <t>CHỈNH SỬA THÔNG TIN CÁ NHÂN</t>
   </si>
+  <si>
+    <t>1. Để trống Tên người dùng
+2. Để trống giới tính
+3. Để trống Mô tả thông tin
+4. Để trống Mật khẩu
+5. Để trống Nhập lại mật khẩu
+6. Không Upload Ảnh
+7. Click nút Cập nhật</t>
+  </si>
+  <si>
+    <t>1. Nhập Tên người dùng
+2. Chọn Giới tính
+4. Để trống Mô tả thông tin
+5. Để trống Mật khẩu
+6. Để trống Nhập lại mật khẩu
+7. Không Upload Ảnh
+8. Click nút Cập nhật</t>
+  </si>
+  <si>
+    <t>1. Nhập đúng Tên người dùng
+2. Chọn Giới tính
+4. Nhập đúng Mô tả thông tin
+5. Để trống Mật khẩu
+6. Để trống Nhập lại mật khẩu
+7. Không Upload Ảnh
+8. Click nút Cập nhật</t>
+  </si>
+  <si>
+    <t>1. Nhập Tên người dùng
+2. Chọn Giới tính
+3. Nhập đúng Mô tả thông tin
+4. Nhập đúng Mật khẩu
+5. Nhập đúng Nhập lại mật khẩu
+6. Upload Ảnh
+7. Click nút Cập nhật</t>
+  </si>
+  <si>
+    <t>1. Nhập đúng Tên người dùng
+2. Chọn Giới tính
+3. Nhập đúng Mô tả thông tin
+4. Nhập đúng Mật khẩu
+5. Nhập đúng Nhập lại mật khẩu
+6. Không Upload Ảnh
+7. Click nút Cập nhật</t>
+  </si>
+  <si>
+    <t>1. Nhập Tên người dùng
+2. Chọn Giới tính
+3. Để trống Mô tả thông tin
+4. Để trống Mật khẩu
+5. Để trống Nhập lại mật khẩu
+6. Không Upload Ảnh
+7. Click nút Cập nhật</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -567,7 +546,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -602,7 +581,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -811,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -831,7 +810,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -896,8 +875,8 @@
         <v>10</v>
       </c>
       <c r="B3" s="7">
-        <f>COUNTIF(H9:H18,"Pass")</f>
-        <v>5</v>
+        <f>COUNTIF(H9:H17,"Pass")</f>
+        <v>9</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -929,7 +908,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="7">
-        <f>COUNTIF(H9:H18,"Fail")</f>
+        <f>COUNTIF(H9:H17,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C4" s="3"/>
@@ -1127,7 +1106,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>2</v>
       </c>
@@ -1135,10 +1114,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="7">
@@ -1169,16 +1148,16 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="18" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="7">
@@ -1209,16 +1188,16 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="18" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="7">
@@ -1251,14 +1230,14 @@
     </row>
     <row r="13" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="7">
@@ -1291,21 +1270,25 @@
     </row>
     <row r="14" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="18" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7">
+        <v>3</v>
+      </c>
       <c r="G14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1325,23 +1308,27 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="18" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7">
+        <v>3</v>
+      </c>
       <c r="G15" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1361,23 +1348,27 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7">
+        <v>3</v>
+      </c>
       <c r="G16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1397,23 +1388,27 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>3</v>
+      </c>
       <c r="G17" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1433,23 +1428,15 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="102" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
-        <v>10</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="7"/>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1581,7 +1568,7 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
@@ -28601,65 +28588,37 @@
       <c r="Y987" s="1"/>
       <c r="Z987" s="1"/>
     </row>
-    <row r="988" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A988" s="6"/>
-      <c r="B988" s="1"/>
-      <c r="C988" s="3"/>
-      <c r="D988" s="3"/>
-      <c r="E988" s="1"/>
-      <c r="F988" s="6"/>
-      <c r="G988" s="6"/>
-      <c r="H988" s="6"/>
-      <c r="I988" s="1"/>
-      <c r="J988" s="1"/>
-      <c r="K988" s="1"/>
-      <c r="L988" s="1"/>
-      <c r="M988" s="1"/>
-      <c r="N988" s="1"/>
-      <c r="O988" s="1"/>
-      <c r="P988" s="1"/>
-      <c r="Q988" s="1"/>
-      <c r="R988" s="1"/>
-      <c r="S988" s="1"/>
-      <c r="T988" s="1"/>
-      <c r="U988" s="1"/>
-      <c r="V988" s="1"/>
-      <c r="W988" s="1"/>
-      <c r="X988" s="1"/>
-      <c r="Y988" s="1"/>
-      <c r="Z988" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B10:B18"/>
+    <mergeCell ref="B10:B17"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:A6 H9:H18">
+  <conditionalFormatting sqref="A3:A6 H9:H17">
     <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH(("Completed"),(A3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A6 H9:H18">
+  <conditionalFormatting sqref="A3:A6 H9:H17">
     <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(A3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A6 H9:H18">
+  <conditionalFormatting sqref="A3:A6 H9:H17">
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="QA">
       <formula>NOT(ISERROR(SEARCH(("QA"),(A3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A6 H9:H18">
+  <conditionalFormatting sqref="A3:A6 H9:H17">
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Not Yet Fixed">
       <formula>NOT(ISERROR(SEARCH(("Not Yet Fixed"),(A3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A6 H9:H18">
+  <conditionalFormatting sqref="A3:A6 H9:H17">
     <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="Reject">
       <formula>NOT(ISERROR(SEARCH(("Reject"),(A3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:H18">
+  <conditionalFormatting sqref="H9:H17">
     <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Loại bỏ">
       <formula>NOT(ISERROR(SEARCH("Loại bỏ",H9)))</formula>
     </cfRule>
@@ -28679,7 +28638,7 @@
       <formula>NOT(ISERROR(SEARCH("Đã hoàn thành",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:H18">
+  <conditionalFormatting sqref="H9:H17">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",H9)))</formula>
     </cfRule>
@@ -28688,11 +28647,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="F9:F18">
+    <dataValidation type="list" allowBlank="1" sqref="A3:A4 H9:H17">
+      <formula1>"Pass, Fail"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="F9:F17">
       <formula1>"1,2,3"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="A3:A4 H9:H18">
-      <formula1>"Pass, Fail"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>